<commit_message>
Working on logicComparator.py code. The code now is more streamlined and works for Platelet Match and WBC trial datasets.
</commit_message>
<xml_diff>
--- a/SMC Challenge 6/eligibility criteria/Dataset1_Platelets_Trials_First.xlsx
+++ b/SMC Challenge 6/eligibility criteria/Dataset1_Platelets_Trials_First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\ClinicalTrialChallenge\SMC Challenge 6\eligibility criteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A085E6F-66DD-4EC9-8230-8BBBB1053BCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D70F82-CE15-4C02-A41E-7F75C4005FB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2923,9 +2923,6 @@
     <t>C51951&gt;100000 or (C51951&lt;=100000 and C3208=1)</t>
   </si>
   <si>
-    <t>(C51951&gt;=70000 and (C12431=1 and C96278&lt;50) or C51951&gt;=50000 and (C12431=1 and C96278&gt;=50)</t>
-  </si>
-  <si>
     <t>C51951&gt;=75000 or (C51951&lt;75000 and C9279=1)</t>
   </si>
   <si>
@@ -2936,6 +2933,9 @@
   </si>
   <si>
     <t>inclusion_indicator</t>
+  </si>
+  <si>
+    <t>C51951&gt;=70000 and (C12431=1 and C96278&lt;50) or C51951&gt;=50000 and (C12431=1 and C96278&gt;=50)</t>
   </si>
 </sst>
 </file>
@@ -3376,10 +3376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -3403,7 +3404,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -3438,7 +3439,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>582</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>585</v>
       </c>
@@ -3558,7 +3559,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>588</v>
       </c>
@@ -3572,7 +3573,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>591</v>
       </c>
@@ -3586,7 +3587,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>594</v>
       </c>
@@ -3646,7 +3647,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>597</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>600</v>
       </c>
@@ -3697,7 +3698,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>603</v>
       </c>
@@ -3711,7 +3712,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>606</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>609</v>
       </c>
@@ -3762,7 +3763,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>612</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>615</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>618</v>
       </c>
@@ -3873,7 +3874,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>621</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>624</v>
       </c>
@@ -3901,7 +3902,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>627</v>
       </c>
@@ -3915,7 +3916,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>630</v>
       </c>
@@ -3929,7 +3930,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>633</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>636</v>
       </c>
@@ -4003,7 +4004,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>639</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>642</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>645</v>
       </c>
@@ -4045,7 +4046,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>648</v>
       </c>
@@ -4059,7 +4060,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>651</v>
       </c>
@@ -4073,7 +4074,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>654</v>
       </c>
@@ -4087,7 +4088,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>657</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>660</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>663</v>
       </c>
@@ -4333,7 +4334,7 @@
         <v>573</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4359,7 +4360,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>666</v>
       </c>
@@ -4373,7 +4374,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>669</v>
       </c>
@@ -4387,7 +4388,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>672</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>675</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>678</v>
       </c>
@@ -4498,7 +4499,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>681</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>684</v>
       </c>
@@ -4549,7 +4550,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>687</v>
       </c>
@@ -4586,7 +4587,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>690</v>
       </c>
@@ -4620,7 +4621,7 @@
         <v>112</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4646,7 +4647,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>693</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>696</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>699</v>
       </c>
@@ -4780,7 +4781,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>702</v>
       </c>
@@ -4794,7 +4795,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>705</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>708</v>
       </c>
@@ -5006,7 +5007,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>711</v>
       </c>
@@ -5043,7 +5044,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>714</v>
       </c>
@@ -5241,7 +5242,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>717</v>
       </c>
@@ -5278,7 +5279,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>720</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>723</v>
       </c>
@@ -5375,7 +5376,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>726</v>
       </c>
@@ -5435,7 +5436,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>729</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>732</v>
       </c>
@@ -5509,7 +5510,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>735</v>
       </c>
@@ -5523,7 +5524,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>738</v>
       </c>
@@ -5606,7 +5607,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>741</v>
       </c>
@@ -5689,7 +5690,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>744</v>
       </c>
@@ -5703,7 +5704,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>747</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>750</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>753</v>
       </c>
@@ -5834,10 +5835,10 @@
         <v>530</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>756</v>
       </c>
@@ -5851,7 +5852,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>759</v>
       </c>
@@ -5865,7 +5866,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>762</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>765</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>768</v>
       </c>
@@ -5953,7 +5954,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>771</v>
       </c>
@@ -5967,7 +5968,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>774</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>777</v>
       </c>
@@ -6087,7 +6088,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>780</v>
       </c>
@@ -6239,7 +6240,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>783</v>
       </c>
@@ -6253,7 +6254,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>786</v>
       </c>
@@ -6267,7 +6268,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>789</v>
       </c>
@@ -6304,7 +6305,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>792</v>
       </c>
@@ -6364,7 +6365,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>795</v>
       </c>
@@ -6378,7 +6379,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>798</v>
       </c>
@@ -6599,7 +6600,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>801</v>
       </c>
@@ -6659,7 +6660,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>804</v>
       </c>
@@ -6719,7 +6720,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>807</v>
       </c>
@@ -6733,7 +6734,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>810</v>
       </c>
@@ -6793,7 +6794,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>813</v>
       </c>
@@ -6830,7 +6831,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>816</v>
       </c>
@@ -6844,7 +6845,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>819</v>
       </c>
@@ -6950,7 +6951,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>822</v>
       </c>
@@ -7010,7 +7011,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>825</v>
       </c>
@@ -7047,7 +7048,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>828</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>831</v>
       </c>
@@ -7075,7 +7076,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>834</v>
       </c>
@@ -7089,7 +7090,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="195" spans="1:7" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" s="3" customFormat="1" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>837</v>
       </c>
@@ -7129,7 +7130,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>840</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>843</v>
       </c>
@@ -7249,7 +7250,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>846</v>
       </c>
@@ -7332,7 +7333,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
         <v>849</v>
       </c>
@@ -7392,7 +7393,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
         <v>852</v>
       </c>
@@ -7452,7 +7453,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>855</v>
       </c>
@@ -7466,7 +7467,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>858</v>
       </c>
@@ -7572,7 +7573,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>861</v>
       </c>
@@ -7586,7 +7587,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
         <v>864</v>
       </c>
@@ -7669,7 +7670,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
         <v>867</v>
       </c>
@@ -7729,7 +7730,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
         <v>870</v>
       </c>
@@ -7812,7 +7813,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
         <v>873</v>
       </c>
@@ -7849,7 +7850,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
         <v>876</v>
       </c>
@@ -7863,7 +7864,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="4" t="s">
         <v>879</v>
       </c>
@@ -7900,7 +7901,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
         <v>882</v>
       </c>
@@ -8029,7 +8030,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
         <v>885</v>
       </c>
@@ -8063,7 +8064,7 @@
         <v>530</v>
       </c>
       <c r="G243" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="244" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8112,7 +8113,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>888</v>
       </c>
@@ -8126,7 +8127,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
         <v>891</v>
       </c>
@@ -8163,7 +8164,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
         <v>894</v>
       </c>
@@ -8269,7 +8270,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
         <v>897</v>
       </c>
@@ -8283,7 +8284,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
         <v>900</v>
       </c>
@@ -8297,7 +8298,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
         <v>903</v>
       </c>
@@ -8334,7 +8335,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
         <v>906</v>
       </c>
@@ -8394,7 +8395,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
         <v>909</v>
       </c>
@@ -8408,7 +8409,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
         <v>912</v>
       </c>
@@ -8422,7 +8423,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
         <v>915</v>
       </c>
@@ -8436,7 +8437,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
         <v>918</v>
       </c>
@@ -8450,7 +8451,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
         <v>921</v>
       </c>
@@ -8487,7 +8488,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>924</v>
       </c>
@@ -8524,7 +8525,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
         <v>927</v>
       </c>
@@ -8538,7 +8539,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>930</v>
       </c>
@@ -8552,7 +8553,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>933</v>
       </c>
@@ -8612,7 +8613,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
         <v>936</v>
       </c>
@@ -8649,7 +8650,14 @@
         <v>943</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="277" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="278" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="279" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="280" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="281" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="282" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="283" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="286" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
     <row r="287" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
     <row r="288" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
@@ -8709,7 +8717,13 @@
     <row r="342" ht="15" x14ac:dyDescent="0.25"/>
     <row r="343" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:G283" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G283" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>